<commit_message>
cnage path images to root folder
</commit_message>
<xml_diff>
--- a/xls/tm-mas.xlsx
+++ b/xls/tm-mas.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TM-MAS-RAD\radar-technologique\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="-75" yWindow="-465" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,18 +17,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="85">
   <si>
     <t>name</t>
   </si>
@@ -118,9 +123,6 @@
     <t>Splunk</t>
   </si>
   <si>
-    <t>Stack ELK</t>
-  </si>
-  <si>
     <t>Node.js</t>
   </si>
   <si>
@@ -139,34 +141,13 @@
     <t>WebStorm</t>
   </si>
   <si>
-    <t>Atom</t>
-  </si>
-  <si>
     <t>Flyway</t>
   </si>
   <si>
     <t>TRUE</t>
   </si>
   <si>
-    <t>asda</t>
-  </si>
-  <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>adsds</t>
-  </si>
-  <si>
     <t>topic</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
   <si>
     <t>Backend solide permettant d'utiliser les compétences WEB des développeurs. Projet toujours maintenu. En surveillance, car Electron parait mieux maintenu.</t>
@@ -271,9 +252,6 @@
     <t>L'utilisation des version de Java en dessous de 8 est à proscrire pour les nouveaux projets.</t>
   </si>
   <si>
-    <t>Les containers d'applications embarqués représente une alternative aux lourds déploiement sur les serveurs applicatifs.</t>
-  </si>
-  <si>
     <t>Outre le fait que les Machines Virtuelles présentent de réelles avanatges pour un evironnement de développement, il y lieu également de s'assurer que certains points critiques soient optimaux dans ce contexte (RAM, accès disques). Le non support de Docker en font d'office une technologie à exclure pour le poste développeur.</t>
   </si>
   <si>
@@ -281,13 +259,50 @@
   </si>
   <si>
     <t>Gestionnaire de source décentralisée. Offre des performances de travail plus performante que SVN.</t>
+  </si>
+  <si>
+    <t>Flyway est un outil permettant d'effectuer des migrations de données.Il est un sérieux concurrent à Liquibase. Plutôt orienté développeur, il apparait souffrir de moins de fonctionnalités que son grand frère.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebStorm est un IDE fournissant un support pour les projets de type "frontend". </t>
+  </si>
+  <si>
+    <t>norme maintenant validé et complète. Apporte un lot de fonctionnalités nottament le local storage, la géolocalisation, l'allégement du code, et toutes les nouvelles balises et attributs.</t>
+  </si>
+  <si>
+    <t>Dropwizard est une combinaison  de plusieurs outils et frameworks Java légers, dont beaucoup mériteraient d'être mentionnés de leur propre chef. 
+Le package incorpore plusieurs composants intéressants, notamment un serveur HTTP intégré, la prise en charge des points de terminaison RESTful, des métriques opérationnelles et des vérifications d'intégrité intégrées, ainsi que des déploiements simples. Dropwizard est le bon outil pour le bon job, vous permettant de vous concentrer sur la complexité essentielle d'un problème plutôt que sur la plomberie. Déjà utilisé sur un projet en production son utilité et ses fonctionnalités doivent toutefois être encore étudier en profondeur.</t>
+  </si>
+  <si>
+    <t>Spring est bien plus qu'un framework, c'est un écosystème complet fournissant toute ce que la stack JEE fournit. Spring en est un concurrent direct.</t>
+  </si>
+  <si>
+    <t>Spring boot et ses librairies starter fournissent une tuyauterie Spring et des mécanismes d'autoconfiguration très productif. Attention toutefois à garder la maitrise des dépendances.</t>
+  </si>
+  <si>
+    <t>Jquery est utilisé sur plusieurs projets. C'est une librairie qui à encore du sens sur les projets "old-school". Pour les nouveaux projets, il n'y a plus d'intérêt à l'utiliser spécifiquement.</t>
+  </si>
+  <si>
+    <t>Node.js en tant que plateforme à encore besoin d'ètre étudier pour en ressortir les fonctionnalités et les besoins qu'il pourrait combler.</t>
+  </si>
+  <si>
+    <t>ElasticSearch</t>
+  </si>
+  <si>
+    <t>ElasticSearch est la référence en matière de moteur d'indexation. Ses possibilités complète sont encore trop peu utilisés et cela nécessite une montée en compétences afin d'en saisir les tenants et les aboutissants.</t>
+  </si>
+  <si>
+    <t>Logstash</t>
+  </si>
+  <si>
+    <t>Logstatsh est un ETL (Extract Transform Load) compagnon idéal de ElastiSearch. Très gourmand en ressources son utilité doit encore être éprouvée.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -316,6 +331,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -343,13 +364,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -365,6 +390,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -694,20 +722,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="142.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17">
+    <row r="1" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -740,24 +768,24 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="112">
+    <row r="2" spans="1:19" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -773,24 +801,24 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="112">
+    <row r="3" spans="1:19" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -806,24 +834,24 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="17">
+    <row r="4" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -839,7 +867,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="64">
+    <row r="5" spans="1:19" ht="66" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -847,16 +875,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -872,7 +900,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="17">
+    <row r="6" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -880,15 +908,17 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -903,24 +933,24 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="17">
+    <row r="7" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -936,23 +966,25 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="17">
+    <row r="8" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -967,24 +999,24 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="17">
+    <row r="9" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1000,24 +1032,24 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" ht="17">
+    <row r="10" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>47</v>
+      <c r="F10" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1033,24 +1065,24 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="17">
+    <row r="11" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>47</v>
+        <v>67</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1066,24 +1098,24 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="17">
+    <row r="12" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1099,7 +1131,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="17">
+    <row r="13" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1107,16 +1139,16 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>47</v>
+      <c r="F13" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1132,24 +1164,24 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="17">
+    <row r="14" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1165,24 +1197,24 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="17">
+    <row r="15" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1198,24 +1230,24 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="17">
+    <row r="16" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>47</v>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1231,24 +1263,24 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="17">
+    <row r="17" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
+      <c r="F17" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1264,24 +1296,24 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="17">
+    <row r="18" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1297,7 +1329,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="17">
+    <row r="19" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1305,7 +1337,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>5</v>
@@ -1313,8 +1345,8 @@
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>47</v>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1330,15 +1362,15 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="17">
+    <row r="20" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>5</v>
@@ -1346,13 +1378,13 @@
       <c r="E20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>47</v>
+      <c r="F20" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1365,7 +1397,7 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" ht="17">
+    <row r="21" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1373,16 +1405,16 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1398,24 +1430,24 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" ht="17">
+    <row r="22" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1431,24 +1463,24 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" ht="17">
+    <row r="23" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1464,24 +1496,24 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" ht="17">
+    <row r="24" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1497,25 +1529,23 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" ht="17">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
+    <row r="25" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="3"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1530,24 +1560,24 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" ht="17">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
+    <row r="26" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>47</v>
+      <c r="D26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1563,24 +1593,24 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" ht="17">
+    <row r="27" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1596,24 +1626,24 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" ht="17">
+    <row r="28" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1629,24 +1659,24 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" ht="17">
+    <row r="29" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1662,24 +1692,24 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" ht="17">
+    <row r="30" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1695,24 +1725,24 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" ht="17">
+    <row r="31" spans="1:19" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1728,24 +1758,24 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" ht="17">
+    <row r="32" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>47</v>
+      <c r="E32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -1761,24 +1791,24 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" ht="17">
+    <row r="33" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>47</v>
+        <v>73</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1796,7 +1826,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1829,56 +1859,56 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add specification and command patterns
</commit_message>
<xml_diff>
--- a/xls/tm-mas.xlsx
+++ b/xls/tm-mas.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -389,12 +389,57 @@
   <si>
     <t>Pratique de tests basé sur les contrats fournis par les API. Presque une évidence afin de gérer le cycle de vie des API (et l'évolution desdites API)</t>
   </si>
+  <si>
+    <t>Nginx</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nginx</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">est un logiciel libre de serveur Web (ou HTTP) ainsi qu'un proxy inverse. Nginx est un système asynchrone (en) par opposition aux serveurs synchrones où chaque requête est traitée par un processus dédié. Au lieu d'exploiter une architecture parallèle et un multiplexage temporel des tâches par le système d'exploitation, Nginx utilise les changements d'état pour gérer plusieurs connexions en même temps ; le traitement de chaque requête est découpé en de nombreuses mini-tâches et permet ainsi de réaliser un multiplexage efficace entre les connexions. </t>
+    </r>
+  </si>
+  <si>
+    <t>Pattern Spécifications</t>
+  </si>
+  <si>
+    <t>03.18</t>
+  </si>
+  <si>
+    <t>Le pattern specification permet une gestion explicite des règles métiers. Il convient bien à la démarche DDD, nottament avec son aspect descriptif.</t>
+  </si>
+  <si>
+    <t>Command Pattern</t>
+  </si>
+  <si>
+    <t>Le commande pattern permet d'implémenter les aspects commadn/event publishing.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -440,6 +485,36 @@
       <color rgb="FF212121"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -467,7 +542,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -484,6 +559,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -830,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -2256,6 +2338,66 @@
         <v>52</v>
       </c>
     </row>
+    <row r="50" spans="1:6" ht="16.5">
+      <c r="A50" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16.5">
+      <c r="A51" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16.5">
+      <c r="A52" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2266,13 +2408,13 @@
           <x14:formula1>
             <xm:f>Feuil2!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B49</xm:sqref>
+          <xm:sqref>B2:B52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Feuil2!$A$8:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C49</xm:sqref>
+          <xm:sqref>C2:C52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add excel sprint 3
</commit_message>
<xml_diff>
--- a/xls/tm-mas.xlsx
+++ b/xls/tm-mas.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="133">
   <si>
     <t>name</t>
   </si>
@@ -429,9 +429,6 @@
     <t>L'aspect volatile de Eclipse, en font un outil qui reste universellement reconnu pour une multitude de langages. Toutefois, la tendance est d'utiliser des IDE spécialisé par lanage, ce qui apporte une plus grande robustesse et une plus grande productivité pour le développeur.</t>
   </si>
   <si>
-    <t>Architecure hexagonale</t>
-  </si>
-  <si>
     <r>
       <t>Le pattern d'archiecture hexagonale, ou architecture en oignon, représente un style d'architecture qui répond parfaitement aux problématiques de la méthode &lt;i&gt;Domain Driven Design&lt;/i&gt;.</t>
     </r>
@@ -453,12 +450,42 @@
   <si>
     <t>Le commande pattern permet d'implémenter les aspects command/event publishing.</t>
   </si>
+  <si>
+    <t>Architecture hexagonale</t>
+  </si>
+  <si>
+    <t>Retrofit</t>
+  </si>
+  <si>
+    <t>Retrofit est un client Java pour les appels sur des API Rest. Il apparait comme un des candidats à utiliser pour les appels sur des servcies web de type REST.</t>
+  </si>
+  <si>
+    <t>sprint3</t>
+  </si>
+  <si>
+    <t>Feign</t>
+  </si>
+  <si>
+    <t>Feign est le concurrent direct de Retrofit. Toutefsois son intégration avec Spring cloud le rendent potentiellement plus adapté à une utilisation dans le cadre d'une architecture distribuée</t>
+  </si>
+  <si>
+    <t>Eureka</t>
+  </si>
+  <si>
+    <t>Spring Zuul gateway</t>
+  </si>
+  <si>
+    <t>Eureka est le composant "Service Discovery", utilisé par la stack Spring Cloud. Il fait partie de la stack Open Source Netflix/OSS</t>
+  </si>
+  <si>
+    <t>Zuul est le composant utilisé par Spring Cloud pour les aspects de Gateway API. Il fait partie de la stack open source Netflix/OSS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -555,6 +582,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -582,7 +621,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,6 +649,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -955,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -2403,7 +2444,7 @@
     </row>
     <row r="51" spans="1:6" ht="16.5">
       <c r="A51" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>45</v>
@@ -2435,7 +2476,7 @@
         <v>37</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>118</v>
@@ -2443,7 +2484,7 @@
     </row>
     <row r="53" spans="1:6" ht="16.5">
       <c r="A53" s="14" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>40</v>
@@ -2455,10 +2496,90 @@
         <v>37</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F53" s="16" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16.5">
+      <c r="A54" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2477,7 +2598,7 @@
           <x14:formula1>
             <xm:f>Feuil2!$A$8:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C53</xm:sqref>
+          <xm:sqref>C2:C54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add sprint 4 technologies
</commit_message>
<xml_diff>
--- a/xls/tm-mas.xlsx
+++ b/xls/tm-mas.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="139">
   <si>
     <t>name</t>
   </si>
@@ -480,12 +480,30 @@
   <si>
     <t>Zuul est le composant utilisé par Spring Cloud pour les aspects de Gateway API. Il fait partie de la stack open source Netflix/OSS</t>
   </si>
+  <si>
+    <t>sprint4</t>
+  </si>
+  <si>
+    <t>Kong API Gateway</t>
+  </si>
+  <si>
+    <t>API Gateway Open Souce et haute performance. Basé sur nGinx. Implémentation minimale mais essentielles d'une Gateway API.</t>
+  </si>
+  <si>
+    <t>Guava</t>
+  </si>
+  <si>
+    <t>Adopeter</t>
+  </si>
+  <si>
+    <t>Librairie fourni par Google proposant toute une panoplie d'outils facilitant la vie du dévelopeur (traitement des collections, validations des paramètres, etc..)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -594,6 +612,13 @@
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -621,7 +646,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -651,6 +676,7 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -996,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -2580,6 +2606,46 @@
       </c>
       <c r="F57" s="17" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>